<commit_message>
Dados de calibracao DHT22
</commit_message>
<xml_diff>
--- a/Calibração DHT-22.xlsx
+++ b/Calibração DHT-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Estacao_meteorologica\Estacao_Meteorologica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06960B0-7B47-4848-AFEA-09F04E42D0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{375EC815-5555-4ECC-9E12-E33E76291F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,43 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Medições da Temperatura</t>
-  </si>
-  <si>
-    <r>
-      <t>T (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C)</t>
-    </r>
-  </si>
-  <si>
-    <t>LM35 (V)</t>
-  </si>
-  <si>
-    <t>Vmed(V)</t>
   </si>
   <si>
     <t>Calibração do LM35</t>
@@ -80,9 +46,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Temp.  [°C]</t>
   </si>
   <si>
     <r>
@@ -218,9 +181,6 @@
     </r>
   </si>
   <si>
-    <t>Vmed. [V]</t>
-  </si>
-  <si>
     <r>
       <t>Δ (</t>
     </r>
@@ -272,52 +232,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Compr. (cm) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>versus</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Temp. (°C) :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> f (x) = a.x + b</t>
-    </r>
-  </si>
-  <si>
-    <t>-b/a (°C)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> f -1 (y) = 4,6792.y - 8,7631</t>
   </si>
   <si>
     <t xml:space="preserve">nro de leituras (n) : </t>
-  </si>
-  <si>
-    <t>MMq Temp. [°C]</t>
   </si>
   <si>
     <r>
@@ -345,71 +263,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>C)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Temp. (°C) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>versus</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Vmed. (V)  :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  f </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (y) = (1/a).y - (b/a)</t>
     </r>
   </si>
   <si>
@@ -447,11 +300,38 @@
     </r>
   </si>
   <si>
-    <t>1/a (°C/V)</t>
+    <t>Incerteza  Padrão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desvio Padrão </t>
+  </si>
+  <si>
+    <t>Incerteza tipoA(V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incerteza Padrão </t>
+  </si>
+  <si>
+    <t>DHT22 (UR%)</t>
+  </si>
+  <si>
+    <t>URmed(UR%)</t>
+  </si>
+  <si>
+    <t>Incerteza tipoB(UR%)</t>
+  </si>
+  <si>
+    <t>Incerteza tipoB(T)</t>
+  </si>
+  <si>
+    <t>dU/dT</t>
+  </si>
+  <si>
+    <t>UR(%) padrão</t>
   </si>
   <si>
     <r>
-      <t>a (V/</t>
+      <t>T (</t>
     </r>
     <r>
       <rPr>
@@ -474,29 +354,145 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>C)</t>
+      <t>C) padrão</t>
     </r>
   </si>
   <si>
-    <t>b (V)</t>
+    <t>Solução salina</t>
   </si>
   <si>
-    <t>Incerteza  Padrão</t>
+    <t>KOH</t>
   </si>
   <si>
-    <t xml:space="preserve">Desvio Padrão </t>
+    <t>Kac</t>
   </si>
   <si>
-    <t>Incerteza tipoA(V)</t>
+    <t>MgCl2</t>
   </si>
   <si>
-    <t xml:space="preserve">IB adc (V) (conversor analógico digital) </t>
+    <t>Ca(NO3)2</t>
   </si>
   <si>
-    <t>IB LM35</t>
+    <t>NaCl</t>
   </si>
   <si>
-    <t xml:space="preserve">Incerteza Padrão </t>
+    <t>KCl</t>
+  </si>
+  <si>
+    <t>1/a (%/%)</t>
+  </si>
+  <si>
+    <t>-b/a (%)</t>
+  </si>
+  <si>
+    <t>a (%/%)</t>
+  </si>
+  <si>
+    <t>b (%)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">UR(%) DHT22 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>versus</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> UR(%) padrão  :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  f </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (y) = (1/a).y - (b/a)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UR(%) padrão </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>versus</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> UR(%) DHT22:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> f (x) = a.x + b</t>
+    </r>
+  </si>
+  <si>
+    <t>MMq Umidade. [%]</t>
   </si>
 </sst>
 </file>
@@ -606,7 +602,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,12 +641,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99FF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -772,7 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -791,9 +781,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,12 +790,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -816,9 +797,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -863,9 +841,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -896,6 +871,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1082,54 +1060,54 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Plan1!$D$16:$D$21</c:f>
+                <c:f>Plan1!$F$16:$F$21</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>5.5043145607490867E-3</c:v>
+                    <c:v>2.0102100498317195</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.5228998930017606E-3</c:v>
+                    <c:v>2.0003333155585179</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5205002697327034E-3</c:v>
+                    <c:v>2.012530193010226</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.5043751189704608E-3</c:v>
+                    <c:v>2.514040572464971</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4699716539288873E-3</c:v>
+                    <c:v>2.002043400572969</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5.4887896768784769E-3</c:v>
+                    <c:v>2.0040542241499688</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Plan1!$D$16:$D$21</c:f>
+                <c:f>Plan1!$F$16:$F$21</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>5.5043145607490867E-3</c:v>
+                    <c:v>2.0102100498317195</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.5228998930017606E-3</c:v>
+                    <c:v>2.0003333155585179</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5205002697327034E-3</c:v>
+                    <c:v>2.012530193010226</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.5043751189704608E-3</c:v>
+                    <c:v>2.514040572464971</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4699716539288873E-3</c:v>
+                    <c:v>2.002043400572969</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5.4887896768784769E-3</c:v>
+                    <c:v>2.0040542241499688</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1150,54 +1128,54 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Plan1!$B$16:$B$21</c:f>
+              <c:f>Plan1!$D$16:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.87</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.18</c:v>
+                  <c:v>32.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.78</c:v>
+                  <c:v>53.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.48</c:v>
+                  <c:v>75.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53.3</c:v>
+                  <c:v>85.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Plan1!$C$16:$C$21</c:f>
+              <c:f>Plan1!$E$16:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.9100000000000005E-2</c:v>
+                  <c:v>12.016666666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15251666666666666</c:v>
+                  <c:v>22.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25163333333333332</c:v>
+                  <c:v>32.716666666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36720000000000003</c:v>
+                  <c:v>57.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45626666666666665</c:v>
+                  <c:v>73.833333333333329</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5353</c:v>
+                  <c:v>83.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1262,7 +1240,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Temperatura</a:t>
+                  <a:t>UR%</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1379,7 +1357,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>LM35</a:t>
+                  <a:t>UR% DHT22</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1586,7 +1564,37 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
@@ -1595,54 +1603,54 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Plan1!$D$16:$D$21</c:f>
+                <c:f>Plan1!$F$16:$F$21</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>5.5043145607490867E-3</c:v>
+                    <c:v>2.0102100498317195</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.5228998930017606E-3</c:v>
+                    <c:v>2.0003333155585179</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5205002697327034E-3</c:v>
+                    <c:v>2.012530193010226</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.5043751189704608E-3</c:v>
+                    <c:v>2.514040572464971</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4699716539288873E-3</c:v>
+                    <c:v>2.002043400572969</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5.4887896768784769E-3</c:v>
+                    <c:v>2.0040542241499688</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Plan1!$D$16:$D$21</c:f>
+                <c:f>Plan1!$F$16:$F$21</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>5.5043145607490867E-3</c:v>
+                    <c:v>2.0102100498317195</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.5228998930017606E-3</c:v>
+                    <c:v>2.0003333155585179</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5205002697327034E-3</c:v>
+                    <c:v>2.012530193010226</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.5043751189704608E-3</c:v>
+                    <c:v>2.514040572464971</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4699716539288873E-3</c:v>
+                    <c:v>2.002043400572969</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5.4887896768784769E-3</c:v>
+                    <c:v>2.0040542241499688</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1663,54 +1671,54 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Plan1!$B$49:$B$54</c:f>
+              <c:f>Plan1!$D$49:$D$54</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.9100000000000005E-2</c:v>
+                  <c:v>12.016666666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15251666666666666</c:v>
+                  <c:v>22.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25163333333333332</c:v>
+                  <c:v>32.716666666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36720000000000003</c:v>
+                  <c:v>57.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45626666666666665</c:v>
+                  <c:v>73.833333333333329</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5353</c:v>
+                  <c:v>83.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Plan1!$C$49:$C$54</c:f>
+              <c:f>Plan1!$E$49:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.9491651347649368</c:v>
+                  <c:v>9.6981190489752187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.252124876351896</c:v>
+                  <c:v>20.810918454736012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.126694027555384</c:v>
+                  <c:v>31.433704658353026</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.640106251272393</c:v>
+                  <c:v>57.561908615519755</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.513436929602882</c:v>
+                  <c:v>74.60736786152134</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53.387189563705277</c:v>
+                  <c:v>85.020148407076732</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1775,9 +1783,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR" baseline="0"/>
-                  <a:t>Temperatura [°C]. </a:t>
+                  <a:t>UR% DHT22</a:t>
                 </a:r>
-                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1810,7 +1817,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1893,7 +1900,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Vmed.[V].</a:t>
+                  <a:t>UR%</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3129,13 +3136,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>2778</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>203597</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>9921</xdr:rowOff>
@@ -3165,13 +3172,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>521891</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>171251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>252016</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>146248</xdr:rowOff>
@@ -3465,1329 +3472,1113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AG68"/>
+  <dimension ref="B2:Y68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="19.54296875" customWidth="1"/>
-    <col min="7" max="7" width="26.26953125" customWidth="1"/>
-    <col min="9" max="9" width="23.54296875" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" customWidth="1"/>
-    <col min="12" max="12" width="22.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
+    <col min="9" max="9" width="26.26953125" customWidth="1"/>
+    <col min="11" max="11" width="23.54296875" customWidth="1"/>
+    <col min="12" max="12" width="17.6328125" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" customWidth="1"/>
+    <col min="15" max="15" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="46" t="s">
+    <row r="2" spans="2:25" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="U2" s="46" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+    </row>
+    <row r="3" spans="2:25" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="I4" s="3">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3">
+        <v>12</v>
+      </c>
+      <c r="K4" s="4">
+        <f>AVERAGE(E4:J4)</f>
+        <v>12.016666666666666</v>
+      </c>
+      <c r="L4">
+        <f>_xlfn.STDEV.S(E4:J4)</f>
+        <v>7.527726527090782E-2</v>
+      </c>
+      <c r="M4">
+        <f>L4/SQRT(6)</f>
+        <v>3.0731814857642845E-2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>0.1</v>
+      </c>
+      <c r="R4">
+        <f>SQRT(M4^2 +N4^2+(P4 * O4)^2)</f>
+        <v>2.0102100498317195</v>
+      </c>
+      <c r="Y4" s="4"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3">
+        <v>22.7</v>
+      </c>
+      <c r="F5" s="3">
+        <v>22.6</v>
+      </c>
+      <c r="G5" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>22.7</v>
+      </c>
+      <c r="I5" s="3">
+        <v>22.6</v>
+      </c>
+      <c r="J5" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="K5" s="4">
+        <f>AVERAGE(E5:J5)</f>
+        <v>22.599999999999998</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L9" si="0">_xlfn.STDEV.S(E5:J5)</f>
+        <v>8.9442719099991269E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M9" si="1">L5/SQRT(6)</f>
+        <v>3.6514837167010948E-2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>1E-4</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R9" si="2">SQRT(M5^2 +N5^2+(P5 * O5)^2)</f>
+        <v>2.0003333155585179</v>
+      </c>
+      <c r="Y5" s="4"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20.8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>32.9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>32.6</v>
+      </c>
+      <c r="F6" s="3">
+        <v>32.9</v>
+      </c>
+      <c r="G6" s="3">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="I6" s="3">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="J6" s="3">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" ref="K6:K9" si="3">AVERAGE(E6:J6)</f>
+        <v>32.716666666666669</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.24832774042918937</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>0.10137937550497049</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>0.1</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>2.012530193010226</v>
+      </c>
+      <c r="Y6" s="4"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2">
+        <v>53.6</v>
+      </c>
+      <c r="E7" s="3">
+        <v>57.6</v>
+      </c>
+      <c r="F7" s="3">
+        <v>57.4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>57.3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>57.6</v>
+      </c>
+      <c r="I7" s="3">
+        <v>57.7</v>
+      </c>
+      <c r="J7" s="3">
+        <v>58</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="3"/>
+        <v>57.6</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.24494897427831896</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.10000000000000048</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>0.76</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>2.514040572464971</v>
+      </c>
+      <c r="Y7" s="4"/>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="E8" s="3">
+        <v>73.8</v>
+      </c>
+      <c r="F8" s="3">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G8" s="3">
+        <v>74</v>
+      </c>
+      <c r="H8" s="3">
+        <v>73.8</v>
+      </c>
+      <c r="I8" s="3">
+        <v>73.7</v>
+      </c>
+      <c r="J8" s="3">
+        <v>73.8</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="3"/>
+        <v>73.833333333333329</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0.10327955589886501</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>4.2163702135578622E-2</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>0.04</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>2.002043400572969</v>
+      </c>
+      <c r="Y8" s="4"/>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2">
+        <v>85.18</v>
+      </c>
+      <c r="E9" s="3">
+        <v>83.7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>83.8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>83.6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>83.7</v>
+      </c>
+      <c r="I9" s="3">
+        <v>83.8</v>
+      </c>
+      <c r="J9" s="3">
+        <v>83.9</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="3"/>
+        <v>83.75</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.10488088481701732</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>4.2817441928884654E-2</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>0.06</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>2.0040542241499688</v>
+      </c>
+      <c r="Y9" s="4"/>
+    </row>
+    <row r="14" spans="2:25" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D14" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+    </row>
+    <row r="15" spans="2:25" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="D16" s="6">
+        <f>D4</f>
+        <v>7.9</v>
+      </c>
+      <c r="E16" s="4">
+        <f>K4</f>
+        <v>12.016666666666666</v>
+      </c>
+      <c r="F16">
+        <f>R4</f>
+        <v>2.0102100498317195</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D17" s="6">
+        <f t="shared" ref="D17:D21" si="4">D5</f>
+        <v>23</v>
+      </c>
+      <c r="E17" s="4">
+        <f>K5</f>
+        <v>22.599999999999998</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F21" si="5">R5</f>
+        <v>2.0003333155585179</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D18" s="6">
+        <f t="shared" si="4"/>
+        <v>32.9</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" ref="E18:E21" si="6">K6</f>
+        <v>32.716666666666669</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>2.012530193010226</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D19" s="6">
+        <f t="shared" si="4"/>
+        <v>53.6</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="6"/>
+        <v>57.6</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>2.514040572464971</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D20" s="6">
+        <f t="shared" si="4"/>
+        <v>75.099999999999994</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="6"/>
+        <v>73.833333333333329</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>2.002043400572969</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D21" s="6">
+        <f t="shared" si="4"/>
+        <v>85.18</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="6"/>
+        <v>83.75</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>2.0040542241499688</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D34" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="4:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D36" s="32">
+        <f>D16</f>
+        <v>7.9</v>
+      </c>
+      <c r="E36" s="39">
+        <f>E16</f>
+        <v>12.016666666666666</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36">
+        <f>1/(F16^2)</f>
+        <v>0.24746690130195087</v>
+      </c>
+      <c r="H36" s="33">
+        <f>D36/F16^2</f>
+        <v>1.9549885202854118</v>
+      </c>
+      <c r="I36" s="15">
+        <f>D16^2*G36</f>
+        <v>15.444409310254755</v>
+      </c>
+      <c r="J36" s="15">
+        <f>E36/F16^2</f>
+        <v>2.9737272639784424</v>
+      </c>
+      <c r="K36" s="15">
+        <f>D36*E36/F16^2</f>
+        <v>23.492445385429697</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D37" s="32">
+        <f t="shared" ref="D37:E41" si="7">D17</f>
+        <v>23</v>
+      </c>
+      <c r="E37" s="39">
+        <f t="shared" si="7"/>
+        <v>22.599999999999998</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="G37">
+        <f t="shared" ref="G37:G41" si="8">1/(F17^2)</f>
+        <v>0.24991669193685415</v>
+      </c>
+      <c r="H37" s="33">
+        <f t="shared" ref="H37:H41" si="9">D37/F17^2</f>
+        <v>5.7480839145476459</v>
+      </c>
+      <c r="I37" s="15">
+        <f t="shared" ref="I37:I41" si="10">D17^2*G37</f>
+        <v>132.20593003459584</v>
+      </c>
+      <c r="J37" s="15">
+        <f t="shared" ref="J37:J41" si="11">E37/F17^2</f>
+        <v>5.6481172377729036</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K41" si="12">D37*E37/F17^2</f>
+        <v>129.90669646877677</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D38" s="32">
+        <f t="shared" si="7"/>
+        <v>32.9</v>
+      </c>
+      <c r="E38" s="39">
+        <f t="shared" si="7"/>
+        <v>32.716666666666669</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38">
+        <f t="shared" si="8"/>
+        <v>0.24689664632055416</v>
+      </c>
+      <c r="H38" s="33">
+        <f t="shared" si="9"/>
+        <v>8.1228996639462316</v>
+      </c>
+      <c r="I38" s="15">
+        <f>D18^2*G38</f>
+        <v>267.24339894383098</v>
+      </c>
+      <c r="J38" s="15">
+        <f t="shared" si="11"/>
+        <v>8.0776352787874632</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" si="12"/>
+        <v>265.75420067210757</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D39" s="32">
+        <f t="shared" si="7"/>
+        <v>53.6</v>
+      </c>
+      <c r="E39" s="39">
+        <f t="shared" si="7"/>
+        <v>57.6</v>
+      </c>
+      <c r="F39" s="14"/>
+      <c r="G39">
+        <f t="shared" si="8"/>
+        <v>0.15821783431428393</v>
+      </c>
+      <c r="H39" s="33">
+        <f t="shared" si="9"/>
+        <v>8.4804759192456185</v>
+      </c>
+      <c r="I39" s="15">
+        <f t="shared" si="10"/>
+        <v>454.55350927156519</v>
+      </c>
+      <c r="J39" s="15">
+        <f t="shared" si="11"/>
+        <v>9.1133472565027542</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="12"/>
+        <v>488.47541294854761</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D40" s="13">
+        <f t="shared" si="7"/>
+        <v>75.099999999999994</v>
+      </c>
+      <c r="E40" s="39">
+        <f t="shared" si="7"/>
+        <v>73.833333333333329</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40">
+        <f t="shared" si="8"/>
+        <v>0.24948993169520089</v>
+      </c>
+      <c r="H40" s="33">
+        <f t="shared" si="9"/>
+        <v>18.736693870309587</v>
+      </c>
+      <c r="I40" s="15">
+        <f t="shared" si="10"/>
+        <v>1407.1257096602499</v>
+      </c>
+      <c r="J40" s="15">
+        <f t="shared" si="11"/>
+        <v>18.420673290162334</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="12"/>
+        <v>1383.3925640911909</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D41" s="13">
+        <f t="shared" si="7"/>
+        <v>85.18</v>
+      </c>
+      <c r="E41" s="39">
+        <f t="shared" si="7"/>
+        <v>83.75</v>
+      </c>
+      <c r="F41" s="14"/>
+      <c r="G41">
+        <f t="shared" si="8"/>
+        <v>0.24898951754131152</v>
+      </c>
+      <c r="H41" s="33">
+        <f t="shared" si="9"/>
+        <v>21.208927104168918</v>
+      </c>
+      <c r="I41" s="15">
+        <f t="shared" si="10"/>
+        <v>1806.5764107331086</v>
+      </c>
+      <c r="J41" s="15">
+        <f t="shared" si="11"/>
+        <v>20.852872094084841</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="12"/>
+        <v>1776.2476449741469</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="36">
+        <f>SUM(G36:G41)</f>
+        <v>1.4009775231101556</v>
+      </c>
+      <c r="H42" s="17">
+        <f>SUM(H36:H41)</f>
+        <v>64.252068992503411</v>
+      </c>
+      <c r="I42" s="18">
+        <f>SUM(I36:I41)</f>
+        <v>4083.1493679536052</v>
+      </c>
+      <c r="J42" s="18">
+        <f>SUM(J36:J41)</f>
+        <v>65.086372421288743</v>
+      </c>
+      <c r="K42" s="19">
+        <f>SUM(K36:K41)</f>
+        <v>4067.2689645401997</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D43" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="26">
+        <f>COUNT(E36:E41)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="H44" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="21"/>
+      <c r="K44" s="22"/>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="H45" s="9">
+        <f>G42*I42-H42^2</f>
+        <v>1592.0721181870204</v>
+      </c>
+      <c r="I45" s="22"/>
+      <c r="K45" s="22"/>
+    </row>
+    <row r="46" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H46" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D47" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="D48" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I48" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D49" s="39">
+        <f>E36</f>
+        <v>12.016666666666666</v>
+      </c>
+      <c r="E49" s="29">
+        <f>$H$56*D49+$I$56</f>
+        <v>9.6981190489752187</v>
+      </c>
+      <c r="H49" s="35">
+        <f>(1/H45)*(G42*K42-H42*J42)</f>
+        <v>0.95235529292889154</v>
+      </c>
+      <c r="I49" s="34">
+        <f>(1/H45)*(I42*J42-H42*K42)</f>
+        <v>2.7806116589206082</v>
+      </c>
+      <c r="J49" s="47"/>
+      <c r="K49" s="48"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D50" s="39">
+        <f t="shared" ref="D50:D54" si="13">E37</f>
+        <v>22.599999999999998</v>
+      </c>
+      <c r="E50" s="29">
+        <f t="shared" ref="E50:E54" si="14">$H$56*D50+$I$56</f>
+        <v>20.810918454736012</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D51" s="39">
+        <f t="shared" si="13"/>
+        <v>32.716666666666669</v>
+      </c>
+      <c r="E51" s="29">
+        <f t="shared" si="14"/>
+        <v>31.433704658353026</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D52" s="39">
+        <f t="shared" si="13"/>
+        <v>57.6</v>
+      </c>
+      <c r="E52" s="29">
+        <f t="shared" si="14"/>
+        <v>57.561908615519755</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="D53" s="39">
+        <f t="shared" si="13"/>
+        <v>73.833333333333329</v>
+      </c>
+      <c r="E53" s="29">
+        <f t="shared" si="14"/>
+        <v>74.60736786152134</v>
+      </c>
+      <c r="H53" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53" s="49"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D54" s="39">
+        <f t="shared" si="13"/>
+        <v>83.75</v>
+      </c>
+      <c r="E54" s="29">
+        <f t="shared" si="14"/>
+        <v>85.020148407076732</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H55" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I55" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E56">
+        <v>99.625718693830393</v>
+      </c>
+      <c r="H56" s="31">
+        <f xml:space="preserve"> 1/H49</f>
+        <v>1.0500282903081066</v>
+      </c>
+      <c r="I56" s="30">
+        <f xml:space="preserve"> -I49/H49</f>
+        <v>-2.919720906227194</v>
+      </c>
+      <c r="J56" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K56" s="41"/>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="E57">
+        <v>5.7542346897863098E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="H58" s="31"/>
+    </row>
+    <row r="61" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="G61" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <f>1/F16^2</f>
+        <v>0.24746690130195087</v>
+      </c>
+      <c r="H62" s="33">
+        <f>D16/F16^2</f>
+        <v>1.9549885202854118</v>
+      </c>
+      <c r="I62" s="15">
+        <f>H62^2</f>
+        <v>3.8219801144477441</v>
+      </c>
+      <c r="J62" s="15">
+        <f>E62</f>
         <v>0</v>
       </c>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-    </row>
-    <row r="3" spans="2:33" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="V3" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B4" s="2">
-        <v>4.87</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5.0499999999999996E-2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5.16E-2</v>
-      </c>
-      <c r="F4" s="3">
-        <v>4.6199999999999998E-2</v>
-      </c>
-      <c r="G4" s="3">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>4.7300000000000002E-2</v>
-      </c>
-      <c r="I4" s="4">
-        <f>AVERAGE(C4:H4)</f>
-        <v>4.9100000000000005E-2</v>
-      </c>
-      <c r="J4">
-        <f>_xlfn.STDEV.S(C4:H4)</f>
-        <v>2.0089798406156293E-3</v>
-      </c>
-      <c r="K4">
-        <f>J4/SQRT(6)</f>
-        <v>8.2016258550769478E-4</v>
-      </c>
-      <c r="L4">
-        <f>(1.1/1023)*2</f>
-        <v>2.1505376344086021E-3</v>
-      </c>
-      <c r="M4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N4">
-        <f>SQRT(K4^2 +L4^2+M4^2)</f>
-        <v>5.5043145607490867E-3</v>
-      </c>
-      <c r="U4" s="2">
-        <v>4.87</v>
-      </c>
-      <c r="V4" s="3">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="W4" s="3">
-        <v>5.0499999999999996E-2</v>
-      </c>
-      <c r="X4" s="3">
-        <v>5.16E-2</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>4.6199999999999998E-2</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>4.7300000000000002E-2</v>
-      </c>
-      <c r="AB4" s="4">
-        <f t="shared" ref="AB4:AB9" si="0">AVERAGE(V4:AA4)</f>
-        <v>4.9100000000000005E-2</v>
-      </c>
-      <c r="AC4">
-        <f t="shared" ref="AC4:AC9" si="1">_xlfn.STDEV.S(V4:AA4)</f>
-        <v>2.0089798406156293E-3</v>
-      </c>
-      <c r="AD4">
-        <f>AC4/SQRT(6)</f>
-        <v>8.2016258550769478E-4</v>
-      </c>
-      <c r="AE4">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="AF4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AG4">
-        <f>SQRT(AD4^2 +AE4^2+AF4^2)</f>
-        <v>5.5238271756696614E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B5" s="2">
-        <v>15.26</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.15160000000000001</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.15380000000000002</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.15479999999999999</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.1484</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.15380000000000002</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.1527</v>
-      </c>
-      <c r="I5" s="4">
-        <f>AVERAGE(C5:H5)</f>
-        <v>0.15251666666666666</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J9" si="2">_xlfn.STDEV.S(C5:H5)</f>
-        <v>2.2947040477296131E-3</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ref="K5:K9" si="3">J5/SQRT(6)</f>
-        <v>9.3680900460612129E-4</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L9" si="4">(1.1/1023)*2</f>
-        <v>2.1505376344086021E-3</v>
-      </c>
-      <c r="M5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N5">
-        <f t="shared" ref="N5:N9" si="5">SQRT(K5^2 +L5^2+M5^2)</f>
-        <v>5.5228998930017606E-3</v>
-      </c>
-      <c r="U5" s="2">
-        <v>15.26</v>
-      </c>
-      <c r="V5" s="3">
-        <v>0.15160000000000001</v>
-      </c>
-      <c r="W5" s="3">
-        <v>0.15380000000000002</v>
-      </c>
-      <c r="X5" s="3">
-        <v>0.15479999999999999</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>0.1484</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>0.15380000000000002</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>0.1527</v>
-      </c>
-      <c r="AB5" s="4">
-        <f t="shared" si="0"/>
-        <v>0.15251666666666666</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="1"/>
-        <v>2.2947040477296131E-3</v>
-      </c>
-      <c r="AD5">
-        <f t="shared" ref="AD5:AD9" si="6">AC5/SQRT(6)</f>
-        <v>9.3680900460612129E-4</v>
-      </c>
-      <c r="AE5">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="AF5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AG5">
-        <f t="shared" ref="AG5:AG9" si="7">SQRT(AD5^2 +AE5^2+AF5^2)</f>
-        <v>5.5423470760239402E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B6" s="2">
-        <v>25.18</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.25379999999999997</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.25379999999999997</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.2495</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.25159999999999999</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.25269999999999998</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.24840000000000001</v>
-      </c>
-      <c r="I6" s="4">
-        <f t="shared" ref="I6:I9" si="8">AVERAGE(C6:H6)</f>
-        <v>0.25163333333333332</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>2.2597935008904228E-3</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
-        <v>9.2255683353986327E-4</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
-        <v>2.1505376344086021E-3</v>
-      </c>
-      <c r="M6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="5"/>
-        <v>5.5205002697327034E-3</v>
-      </c>
-      <c r="U6" s="2">
-        <v>25.18</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0.25379999999999997</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0.25379999999999997</v>
-      </c>
-      <c r="X6" s="3">
-        <v>0.2495</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>0.25159999999999999</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>0.25269999999999998</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>0.24840000000000001</v>
-      </c>
-      <c r="AB6" s="4">
-        <f t="shared" si="0"/>
-        <v>0.25163333333333332</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="1"/>
-        <v>2.2597935008904228E-3</v>
-      </c>
-      <c r="AD6">
-        <f t="shared" si="6"/>
-        <v>9.2255683353986327E-4</v>
-      </c>
-      <c r="AE6">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="AF6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AG6">
-        <f t="shared" si="7"/>
-        <v>5.5399558762783572E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B7" s="2">
-        <v>36.78</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.36880000000000002</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.36560000000000004</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.36770000000000003</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.36670000000000003</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.36450000000000005</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.36990000000000001</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="8"/>
-        <v>0.36720000000000003</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>2.0099751242241646E-3</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
-        <v>8.2056890833940601E-4</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
-        <v>2.1505376344086021E-3</v>
-      </c>
-      <c r="M7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="5"/>
-        <v>5.5043751189704608E-3</v>
-      </c>
-      <c r="U7" s="2">
-        <v>36.78</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0.36880000000000002</v>
-      </c>
-      <c r="W7" s="3">
-        <v>0.36560000000000004</v>
-      </c>
-      <c r="X7" s="3">
-        <v>0.36770000000000003</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>0.36670000000000003</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>0.36450000000000005</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>0.36990000000000001</v>
-      </c>
-      <c r="AB7" s="4">
-        <f t="shared" si="0"/>
-        <v>0.36720000000000003</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="1"/>
-        <v>2.0099751242241646E-3</v>
-      </c>
-      <c r="AD7">
-        <f t="shared" si="6"/>
-        <v>8.2056890833940601E-4</v>
-      </c>
-      <c r="AE7">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="AF7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AG7">
-        <f t="shared" si="7"/>
-        <v>5.5238875199747984E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B8" s="2">
-        <v>45.48</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.45810000000000001</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.45590000000000003</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="8"/>
-        <v>0.45626666666666665</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>1.3321661558029086E-3</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
-        <v>5.4385455572035371E-4</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="4"/>
-        <v>2.1505376344086021E-3</v>
-      </c>
-      <c r="M8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="5"/>
-        <v>5.4699716539288873E-3</v>
-      </c>
-      <c r="U8" s="2">
-        <v>45.48</v>
-      </c>
-      <c r="V8" s="3">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="W8" s="3">
-        <v>0.45810000000000001</v>
-      </c>
-      <c r="X8" s="3">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>0.45590000000000003</v>
-      </c>
-      <c r="AB8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.45626666666666665</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="1"/>
-        <v>1.3321661558029086E-3</v>
-      </c>
-      <c r="AD8">
-        <f t="shared" si="6"/>
-        <v>5.4385455572035371E-4</v>
-      </c>
-      <c r="AE8">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="AF8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AG8">
-        <f t="shared" si="7"/>
-        <v>5.4896063408752535E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B9" s="2">
-        <v>53.3</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.53549999999999998</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.5333</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.53659999999999997</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.53549999999999998</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.5333</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.53759999999999997</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="8"/>
-        <v>0.5353</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>1.7355114519933177E-3</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="3"/>
-        <v>7.0851958335672871E-4</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="4"/>
-        <v>2.1505376344086021E-3</v>
-      </c>
-      <c r="M9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="5"/>
-        <v>5.4887896768784769E-3</v>
-      </c>
-      <c r="U9" s="2">
-        <v>53.3</v>
-      </c>
-      <c r="V9" s="3">
-        <v>0.53549999999999998</v>
-      </c>
-      <c r="W9" s="3">
-        <v>0.5333</v>
-      </c>
-      <c r="X9" s="3">
-        <v>0.53659999999999997</v>
-      </c>
-      <c r="Y9" s="3">
-        <v>0.53549999999999998</v>
-      </c>
-      <c r="Z9" s="3">
-        <v>0.5333</v>
-      </c>
-      <c r="AA9" s="3">
-        <v>0.53759999999999997</v>
-      </c>
-      <c r="AB9" s="4">
-        <f t="shared" si="0"/>
-        <v>0.5353</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="1"/>
-        <v>1.7355114519933177E-3</v>
-      </c>
-      <c r="AD9">
-        <f t="shared" si="6"/>
-        <v>7.0851958335672871E-4</v>
-      </c>
-      <c r="AE9">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="AF9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AG9">
-        <f t="shared" si="7"/>
-        <v>5.508357286886899E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:33" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-    </row>
-    <row r="15" spans="2:33" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.35">
-      <c r="B16" s="6">
-        <f>B4</f>
-        <v>4.87</v>
-      </c>
-      <c r="C16" s="4">
-        <f>I4</f>
-        <v>4.9100000000000005E-2</v>
-      </c>
-      <c r="D16">
-        <f>N4</f>
-        <v>5.5043145607490867E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="6">
-        <f t="shared" ref="B17:B21" si="9">B5</f>
-        <v>15.26</v>
-      </c>
-      <c r="C17" s="4">
-        <f>I5</f>
-        <v>0.15251666666666666</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ref="D17:D21" si="10">N5</f>
-        <v>5.5228998930017606E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="6">
-        <f t="shared" si="9"/>
-        <v>25.18</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" ref="C18:C21" si="11">I6</f>
-        <v>0.25163333333333332</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="10"/>
-        <v>5.5205002697327034E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="6">
-        <f t="shared" si="9"/>
-        <v>36.78</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="11"/>
-        <v>0.36720000000000003</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="10"/>
-        <v>5.5043751189704608E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="6">
-        <f t="shared" si="9"/>
-        <v>45.48</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="11"/>
-        <v>0.45626666666666665</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="10"/>
-        <v>5.4699716539288873E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="6">
-        <f t="shared" si="9"/>
-        <v>53.3</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="11"/>
-        <v>0.5353</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="10"/>
-        <v>5.4887896768784769E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B34" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="2:9" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B36" s="37">
-        <f>B16</f>
-        <v>4.87</v>
-      </c>
-      <c r="C36" s="17">
-        <f>C16</f>
-        <v>4.9100000000000005E-2</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="E36">
-        <f>1/(D16^2)</f>
-        <v>33006.046712337105</v>
-      </c>
-      <c r="F36" s="38">
-        <f>B36/D16^2</f>
-        <v>160739.44748908171</v>
-      </c>
-      <c r="G36" s="19">
-        <f>B16^2*E36</f>
-        <v>782801.10927182797</v>
-      </c>
-      <c r="H36" s="19">
-        <f>C36/D16^2</f>
-        <v>1620.5968935757521</v>
-      </c>
-      <c r="I36" s="19">
-        <f>B36*C36/D16^2</f>
-        <v>7892.3068717139122</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B37" s="37">
-        <f t="shared" ref="B37:C41" si="12">B17</f>
-        <v>15.26</v>
-      </c>
-      <c r="C37" s="17">
-        <f t="shared" si="12"/>
-        <v>0.15251666666666666</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37">
-        <f t="shared" ref="E37:E41" si="13">1/(D17^2)</f>
-        <v>32784.280531460972</v>
-      </c>
-      <c r="F37" s="38">
-        <f t="shared" ref="F37:F41" si="14">B37/D17^2</f>
-        <v>500288.12091009441</v>
-      </c>
-      <c r="G37" s="19">
-        <f t="shared" ref="G37:G41" si="15">B17^2*E37</f>
-        <v>7634396.7250880403</v>
-      </c>
-      <c r="H37" s="19">
-        <f t="shared" ref="H37:H41" si="16">C37/D17^2</f>
-        <v>5000.1491857233223</v>
-      </c>
-      <c r="I37" s="19">
-        <f t="shared" ref="I37:I41" si="17">B37*C37/D17^2</f>
-        <v>76302.276574137897</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B38" s="37">
-        <f t="shared" si="12"/>
-        <v>25.18</v>
-      </c>
-      <c r="C38" s="17">
-        <f t="shared" si="12"/>
-        <v>0.25163333333333332</v>
-      </c>
-      <c r="D38" s="18"/>
-      <c r="E38">
-        <f t="shared" si="13"/>
-        <v>32812.787737873747</v>
-      </c>
-      <c r="F38" s="38">
-        <f t="shared" si="14"/>
-        <v>826225.99523966096</v>
-      </c>
-      <c r="G38" s="19">
+      <c r="K62" s="15">
+        <f>H62*J62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="G63">
+        <f t="shared" ref="G63:G67" si="15">1/F17^2</f>
+        <v>0.24991669193685415</v>
+      </c>
+      <c r="H63" s="33">
+        <f t="shared" ref="H63:H67" si="16">D17/F17^2</f>
+        <v>5.7480839145476459</v>
+      </c>
+      <c r="I63" s="15">
+        <f t="shared" ref="I63:I67" si="17">H63^2</f>
+        <v>33.040468688681386</v>
+      </c>
+      <c r="J63" s="15">
+        <f t="shared" ref="J63:J67" si="18">E63</f>
+        <v>0</v>
+      </c>
+      <c r="K63" s="15">
+        <f t="shared" ref="K63:K67" si="19">H63*J63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="G64">
         <f t="shared" si="15"/>
-        <v>20804370.56013466</v>
-      </c>
-      <c r="H38" s="19">
+        <v>0.24689664632055416</v>
+      </c>
+      <c r="H64" s="33">
         <f t="shared" si="16"/>
-        <v>8256.7911544402978</v>
-      </c>
-      <c r="I38" s="19">
+        <v>8.1228996639462316</v>
+      </c>
+      <c r="I64" s="15">
         <f t="shared" si="17"/>
-        <v>207906.00126880666</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B39" s="37">
-        <f t="shared" si="12"/>
-        <v>36.78</v>
-      </c>
-      <c r="C39" s="17">
-        <f t="shared" si="12"/>
-        <v>0.36720000000000003</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39">
-        <f t="shared" si="13"/>
-        <v>33005.320462237818</v>
-      </c>
-      <c r="F39" s="38">
-        <f t="shared" si="14"/>
-        <v>1213935.686601107</v>
-      </c>
-      <c r="G39" s="19">
+        <v>65.981498950537798</v>
+      </c>
+      <c r="J64" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K64" s="15">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G65">
         <f t="shared" si="15"/>
-        <v>44648554.553188719</v>
-      </c>
-      <c r="H39" s="19">
+        <v>0.15821783431428393</v>
+      </c>
+      <c r="H65" s="33">
         <f t="shared" si="16"/>
-        <v>12119.553673733728</v>
-      </c>
-      <c r="I39" s="19">
+        <v>8.4804759192456185</v>
+      </c>
+      <c r="I65" s="15">
         <f t="shared" si="17"/>
-        <v>445757.18411992653</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B40" s="16">
-        <f t="shared" si="12"/>
-        <v>45.48</v>
-      </c>
-      <c r="C40" s="17">
-        <f t="shared" si="12"/>
-        <v>0.45626666666666665</v>
-      </c>
-      <c r="D40" s="18"/>
-      <c r="E40">
-        <f t="shared" si="13"/>
-        <v>33421.800957683561</v>
-      </c>
-      <c r="F40" s="38">
-        <f t="shared" si="14"/>
-        <v>1520023.5075554482</v>
-      </c>
-      <c r="G40" s="19">
+        <v>71.918471816904812</v>
+      </c>
+      <c r="J65" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K65" s="15">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G66">
         <f t="shared" si="15"/>
-        <v>69130669.123621777</v>
-      </c>
-      <c r="H40" s="19">
+        <v>0.24948993169520089</v>
+      </c>
+      <c r="H66" s="33">
         <f t="shared" si="16"/>
-        <v>15249.253716959085</v>
-      </c>
-      <c r="I40" s="19">
+        <v>18.736693870309587</v>
+      </c>
+      <c r="I66" s="15">
         <f t="shared" si="17"/>
-        <v>693536.0590472992</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="16">
-        <f t="shared" si="12"/>
-        <v>53.3</v>
-      </c>
-      <c r="C41" s="17">
-        <f t="shared" si="12"/>
-        <v>0.5353</v>
-      </c>
-      <c r="D41" s="18"/>
-      <c r="E41">
-        <f t="shared" si="13"/>
-        <v>33193.024078225048</v>
-      </c>
-      <c r="F41" s="38">
-        <f t="shared" si="14"/>
-        <v>1769188.1833693951</v>
-      </c>
-      <c r="G41" s="19">
+        <v>351.06369718969682</v>
+      </c>
+      <c r="J66" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="15">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G67">
         <f t="shared" si="15"/>
-        <v>94297730.173588753</v>
-      </c>
-      <c r="H41" s="19">
+        <v>0.24898951754131152</v>
+      </c>
+      <c r="H67" s="33">
         <f t="shared" si="16"/>
-        <v>17768.225789073869</v>
-      </c>
-      <c r="I41" s="19">
+        <v>21.208927104168918</v>
+      </c>
+      <c r="I67" s="16">
         <f t="shared" si="17"/>
-        <v>947046.4345576372</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="41">
-        <f>SUM(E36:E41)</f>
-        <v>198223.26047981824</v>
-      </c>
-      <c r="F42" s="21">
-        <f>SUM(F36:F41)</f>
-        <v>5990400.9411647879</v>
-      </c>
-      <c r="G42" s="22">
-        <f>SUM(G36:G41)</f>
-        <v>237298522.24489379</v>
-      </c>
-      <c r="H42" s="22">
-        <f>SUM(H36:H41)</f>
-        <v>60014.570413506051</v>
-      </c>
-      <c r="I42" s="23">
-        <f>SUM(I36:I41)</f>
-        <v>2378440.2624395215</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B43" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="30">
-        <f>COUNT(C36:C41)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="F44" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="25"/>
-      <c r="I44" s="26"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="F45" s="10">
-        <f>E42*G42-F42^2</f>
-        <v>11153183350517.547</v>
-      </c>
-      <c r="G45" s="26"/>
-      <c r="I45" s="26"/>
-    </row>
-    <row r="46" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="F46" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B47" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="B48" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B49" s="17">
-        <f>C36</f>
-        <v>4.9100000000000005E-2</v>
-      </c>
-      <c r="C49" s="34">
-        <f>$F$56*B49+$G$56</f>
-        <v>4.9491651347649368</v>
-      </c>
-      <c r="F49" s="40">
-        <f>1/F45*(E42*I42-F42*H42)</f>
-        <v>1.003756874340047E-2</v>
-      </c>
-      <c r="G49" s="39">
-        <f>1/F45*(G42*H42-F42*I42)</f>
-        <v>-5.7758526264389722E-4</v>
-      </c>
-      <c r="H49" s="51"/>
-      <c r="I49" s="52"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B50" s="17">
-        <f t="shared" ref="B50:B54" si="18">C37</f>
-        <v>0.15251666666666666</v>
-      </c>
-      <c r="C50" s="34">
-        <f t="shared" ref="C50:C54" si="19">$F$56*B50+$G$56</f>
-        <v>15.252124876351896</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B51" s="17">
+        <v>449.81858890995096</v>
+      </c>
+      <c r="J67" s="16">
         <f t="shared" si="18"/>
-        <v>0.25163333333333332</v>
-      </c>
-      <c r="C51" s="34">
+        <v>0</v>
+      </c>
+      <c r="K67" s="16">
         <f t="shared" si="19"/>
-        <v>25.126694027555384</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B52" s="17">
-        <f t="shared" si="18"/>
-        <v>0.36720000000000003</v>
-      </c>
-      <c r="C52" s="34">
-        <f t="shared" si="19"/>
-        <v>36.640106251272393</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="B53" s="17">
-        <f t="shared" si="18"/>
-        <v>0.45626666666666665</v>
-      </c>
-      <c r="C53" s="34">
-        <f t="shared" si="19"/>
-        <v>45.513436929602882</v>
-      </c>
-      <c r="F53" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="53"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B54" s="17">
-        <f t="shared" si="18"/>
-        <v>0.5353</v>
-      </c>
-      <c r="C54" s="34">
-        <f t="shared" si="19"/>
-        <v>53.387189563705277</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="F55" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C56">
-        <v>99.625718693830393</v>
-      </c>
-      <c r="F56" s="36">
-        <f xml:space="preserve"> 1/F49</f>
-        <v>99.625718693830407</v>
-      </c>
-      <c r="G56" s="35">
-        <f xml:space="preserve"> -G49/F49</f>
-        <v>5.7542346897863056E-2</v>
-      </c>
-      <c r="H56" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I56" s="45"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="C57">
-        <v>5.7542346897863098E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="F58" s="36"/>
-    </row>
-    <row r="61" spans="2:9" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="E61" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I61" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="E62">
-        <f>1/D16^2</f>
-        <v>33006.046712337105</v>
-      </c>
-      <c r="F62" s="38">
-        <f>B16/D16^2</f>
-        <v>160739.44748908171</v>
-      </c>
-      <c r="G62" s="19">
-        <f>F62^2</f>
-        <v>25837169979.095257</v>
-      </c>
-      <c r="H62" s="19">
-        <f>C62</f>
         <v>0</v>
       </c>
-      <c r="I62" s="19">
-        <f>F62*H62</f>
+    </row>
+    <row r="68" spans="7:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G68">
+        <f>SUM(G62:G67)</f>
+        <v>1.4009775231101556</v>
+      </c>
+      <c r="H68" s="17">
+        <f>SUM(H62:H67)</f>
+        <v>64.252068992503411</v>
+      </c>
+      <c r="I68" s="18">
+        <f>SUM(I62:I67)</f>
+        <v>975.64470567021954</v>
+      </c>
+      <c r="J68" s="18">
+        <f>SUM(J62:J67)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="E63">
-        <f t="shared" ref="E63:E67" si="20">1/D17^2</f>
-        <v>32784.280531460972</v>
-      </c>
-      <c r="F63" s="38">
-        <f t="shared" ref="F63:F67" si="21">B17/D17^2</f>
-        <v>500288.12091009441</v>
-      </c>
-      <c r="G63" s="19">
-        <f t="shared" ref="G63:G67" si="22">F63^2</f>
-        <v>250288203923.75323</v>
-      </c>
-      <c r="H63" s="19">
-        <f t="shared" ref="H63:H67" si="23">C63</f>
+      <c r="K68" s="19">
+        <f>SUM(K62:K67)</f>
         <v>0</v>
       </c>
-      <c r="I63" s="19">
-        <f t="shared" ref="I63:I67" si="24">F63*H63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="E64">
-        <f t="shared" si="20"/>
-        <v>32812.787737873747</v>
-      </c>
-      <c r="F64" s="38">
-        <f t="shared" si="21"/>
-        <v>826225.99523966096</v>
-      </c>
-      <c r="G64" s="19">
-        <f t="shared" si="22"/>
-        <v>682649395209.76831</v>
-      </c>
-      <c r="H64" s="19">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I64" s="19">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="5:9" x14ac:dyDescent="0.35">
-      <c r="E65">
-        <f t="shared" si="20"/>
-        <v>33005.320462237818</v>
-      </c>
-      <c r="F65" s="38">
-        <f t="shared" si="21"/>
-        <v>1213935.686601107</v>
-      </c>
-      <c r="G65" s="19">
-        <f t="shared" si="22"/>
-        <v>1473639851203.7012</v>
-      </c>
-      <c r="H65" s="19">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I65" s="19">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="5:9" x14ac:dyDescent="0.35">
-      <c r="E66">
-        <f t="shared" si="20"/>
-        <v>33421.800957683561</v>
-      </c>
-      <c r="F66" s="38">
-        <f t="shared" si="21"/>
-        <v>1520023.5075554482</v>
-      </c>
-      <c r="G66" s="19">
-        <f t="shared" si="22"/>
-        <v>2310471463521.168</v>
-      </c>
-      <c r="H66" s="19">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I66" s="19">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E67">
-        <f t="shared" si="20"/>
-        <v>33193.024078225048</v>
-      </c>
-      <c r="F67" s="38">
-        <f t="shared" si="21"/>
-        <v>1769188.1833693951</v>
-      </c>
-      <c r="G67" s="20">
-        <f t="shared" si="22"/>
-        <v>3130026828173.9004</v>
-      </c>
-      <c r="H67" s="20">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I67" s="20">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="5:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E68">
-        <f>SUM(E62:E67)</f>
-        <v>198223.26047981824</v>
-      </c>
-      <c r="F68" s="21">
-        <f>SUM(F62:F67)</f>
-        <v>5990400.9411647879</v>
-      </c>
-      <c r="G68" s="22">
-        <f>SUM(G62:G67)</f>
-        <v>7872912912011.3867</v>
-      </c>
-      <c r="H68" s="22">
-        <f>SUM(H62:H67)</f>
-        <v>0</v>
-      </c>
-      <c r="I68" s="23">
-        <f>SUM(I62:I67)</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="U2:AA2"/>
-    <mergeCell ref="V3:AA3"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="F53:I53"/>
+  <mergeCells count="7">
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="H53:K53"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I5:J9 I4" formulaRange="1"/>
+    <ignoredError sqref="K5:L9 K4" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização - Excel da Calibragem
</commit_message>
<xml_diff>
--- a/Calibração DHT-22.xlsx
+++ b/Calibração DHT-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Estacao_meteorologica\Estacao_Meteorologica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{375EC815-5555-4ECC-9E12-E33E76291F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD0185E-5C90-43C7-979A-A0D2F6509759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Medições da Temperatura</t>
   </si>
@@ -46,139 +46,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <r>
-      <t>Sx (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Sx</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Sy (cm)</t>
-  </si>
-  <si>
-    <r>
-      <t>Sxy (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C.cm)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -238,66 +105,7 @@
     <t xml:space="preserve">nro de leituras (n) : </t>
   </si>
   <si>
-    <r>
-      <t>Ssigma (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C)</t>
-    </r>
-  </si>
-  <si>
     <t>Ssigma</t>
-  </si>
-  <si>
-    <t>Sy (V)</t>
-  </si>
-  <si>
-    <r>
-      <t>Sxy (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C.V)</t>
-    </r>
   </si>
   <si>
     <t>Incerteza  Padrão</t>
@@ -494,6 +302,66 @@
   <si>
     <t>MMq Umidade. [%]</t>
   </si>
+  <si>
+    <t>Sx (%)</t>
+  </si>
+  <si>
+    <r>
+      <t>Sx</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (% </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Sy (%)</t>
+  </si>
+  <si>
+    <t>Sxy (% . %)</t>
+  </si>
 </sst>
 </file>
 
@@ -645,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -739,19 +607,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -762,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -805,9 +660,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -875,7 +727,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -896,7 +748,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1065,22 +917,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.0102100498317195</c:v>
+                    <c:v>2.0008609258127974</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.0003333155585179</c:v>
+                    <c:v>2.0003333061850799</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.012530193010226</c:v>
+                    <c:v>2.0031918973922038</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.514040572464971</c:v>
+                    <c:v>2.0382345301755636</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.002043400572969</c:v>
+                    <c:v>2.0005443703596724</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0040542241499688</c:v>
+                    <c:v>2.00068321663709</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1092,22 +944,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.0102100498317195</c:v>
+                    <c:v>2.0008609258127974</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.0003333155585179</c:v>
+                    <c:v>2.0003333061850799</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.012530193010226</c:v>
+                    <c:v>2.0031918973922038</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.514040572464971</c:v>
+                    <c:v>2.0382345301755636</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.002043400572969</c:v>
+                    <c:v>2.0005443703596724</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0040542241499688</c:v>
+                    <c:v>2.00068321663709</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1608,22 +1460,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.0102100498317195</c:v>
+                    <c:v>2.0008609258127974</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.0003333155585179</c:v>
+                    <c:v>2.0003333061850799</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.012530193010226</c:v>
+                    <c:v>2.0031918973922038</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.514040572464971</c:v>
+                    <c:v>2.0382345301755636</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.002043400572969</c:v>
+                    <c:v>2.0005443703596724</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0040542241499688</c:v>
+                    <c:v>2.00068321663709</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1635,22 +1487,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.0102100498317195</c:v>
+                    <c:v>2.0008609258127974</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.0003333155585179</c:v>
+                    <c:v>2.0003333061850799</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.012530193010226</c:v>
+                    <c:v>2.0031918973922038</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.514040572464971</c:v>
+                    <c:v>2.0382345301755636</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.002043400572969</c:v>
+                    <c:v>2.0005443703596724</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0040542241499688</c:v>
+                    <c:v>2.00068321663709</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1703,22 +1555,22 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.6981190489752187</c:v>
+                  <c:v>9.5513194889059019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.810918454736012</c:v>
+                  <c:v>20.64206474024909</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.433704658353026</c:v>
+                  <c:v>31.243769256099995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.561908615519755</c:v>
+                  <c:v>57.320119902171463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.60736786152134</c:v>
+                  <c:v>74.331751201082113</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85.020148407076732</c:v>
+                  <c:v>84.72386683029346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3472,10 +3324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Y68"/>
+  <dimension ref="B2:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61:K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3495,60 +3347,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="2:25" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+        <v>17</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="38" t="s">
-        <v>18</v>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="37" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2">
         <v>25.9</v>
@@ -3590,20 +3442,20 @@
         <v>2</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P4">
         <v>0.1</v>
       </c>
       <c r="R4">
         <f>SQRT(M4^2 +N4^2+(P4 * O4)^2)</f>
-        <v>2.0102100498317195</v>
+        <v>2.0008609258127974</v>
       </c>
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2">
         <v>24</v>
@@ -3645,20 +3497,20 @@
         <v>2</v>
       </c>
       <c r="O5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P5">
         <v>1E-4</v>
       </c>
       <c r="R5">
         <f t="shared" ref="R5:R9" si="2">SQRT(M5^2 +N5^2+(P5 * O5)^2)</f>
-        <v>2.0003333155585179</v>
+        <v>2.0003333061850799</v>
       </c>
       <c r="Y5" s="4"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>20.8</v>
@@ -3700,20 +3552,20 @@
         <v>2</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P6">
         <v>0.1</v>
       </c>
       <c r="R6">
         <f t="shared" si="2"/>
-        <v>2.012530193010226</v>
+        <v>2.0031918973922038</v>
       </c>
       <c r="Y6" s="4"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2">
         <v>23</v>
@@ -3755,20 +3607,20 @@
         <v>2</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P7">
         <v>0.76</v>
       </c>
       <c r="R7">
         <f t="shared" si="2"/>
-        <v>2.514040572464971</v>
+        <v>2.0382345301755636</v>
       </c>
       <c r="Y7" s="4"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2">
         <v>23.5</v>
@@ -3810,20 +3662,20 @@
         <v>2</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P8">
         <v>0.04</v>
       </c>
       <c r="R8">
         <f t="shared" si="2"/>
-        <v>2.002043400572969</v>
+        <v>2.0005443703596724</v>
       </c>
       <c r="Y8" s="4"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2">
         <v>23</v>
@@ -3865,37 +3717,37 @@
         <v>2</v>
       </c>
       <c r="O9">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P9">
         <v>0.06</v>
       </c>
       <c r="R9">
         <f t="shared" si="2"/>
-        <v>2.0040542241499688</v>
+        <v>2.00068321663709</v>
       </c>
       <c r="Y9" s="4"/>
     </row>
     <row r="14" spans="2:25" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="2:25" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.35">
@@ -3909,7 +3761,7 @@
       </c>
       <c r="F16">
         <f>R4</f>
-        <v>2.0102100498317195</v>
+        <v>2.0008609258127974</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.35">
@@ -3923,7 +3775,7 @@
       </c>
       <c r="F17">
         <f t="shared" ref="F17:F21" si="5">R5</f>
-        <v>2.0003333155585179</v>
+        <v>2.0003333061850799</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.35">
@@ -3937,7 +3789,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="5"/>
-        <v>2.012530193010226</v>
+        <v>2.0031918973922038</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.35">
@@ -3951,7 +3803,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="5"/>
-        <v>2.514040572464971</v>
+        <v>2.0382345301755636</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.35">
@@ -3965,7 +3817,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="5"/>
-        <v>2.002043400572969</v>
+        <v>2.0005443703596724</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.35">
@@ -3979,7 +3831,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="5"/>
-        <v>2.0040542241499688</v>
+        <v>2.00068321663709</v>
       </c>
     </row>
     <row r="34" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3998,150 +3850,150 @@
     </row>
     <row r="35" spans="4:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D35" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D36" s="32">
+      <c r="D36" s="31">
         <f>D16</f>
         <v>7.9</v>
       </c>
-      <c r="E36" s="39">
+      <c r="E36" s="38">
         <f>E16</f>
         <v>12.016666666666666</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36">
         <f>1/(F16^2)</f>
-        <v>0.24746690130195087</v>
-      </c>
-      <c r="H36" s="33">
+        <v>0.24978490744081483</v>
+      </c>
+      <c r="H36" s="32">
         <f>D36/F16^2</f>
-        <v>1.9549885202854118</v>
+        <v>1.9733007687824373</v>
       </c>
       <c r="I36" s="15">
         <f>D16^2*G36</f>
-        <v>15.444409310254755</v>
+        <v>15.589076073381255</v>
       </c>
       <c r="J36" s="15">
         <f>E36/F16^2</f>
-        <v>2.9737272639784424</v>
+        <v>3.0015819710804581</v>
       </c>
       <c r="K36" s="15">
         <f>D36*E36/F16^2</f>
-        <v>23.492445385429697</v>
+        <v>23.712497571535618</v>
       </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D37" s="32">
+      <c r="D37" s="31">
         <f t="shared" ref="D37:E41" si="7">D17</f>
         <v>23</v>
       </c>
-      <c r="E37" s="39">
+      <c r="E37" s="38">
         <f t="shared" si="7"/>
         <v>22.599999999999998</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37">
         <f t="shared" ref="G37:G41" si="8">1/(F17^2)</f>
-        <v>0.24991669193685415</v>
-      </c>
-      <c r="H37" s="33">
+        <v>0.24991669427904245</v>
+      </c>
+      <c r="H37" s="32">
         <f t="shared" ref="H37:H41" si="9">D37/F17^2</f>
-        <v>5.7480839145476459</v>
+        <v>5.7480839684179763</v>
       </c>
       <c r="I37" s="15">
         <f t="shared" ref="I37:I41" si="10">D17^2*G37</f>
-        <v>132.20593003459584</v>
+        <v>132.20593127361346</v>
       </c>
       <c r="J37" s="15">
         <f t="shared" ref="J37:J41" si="11">E37/F17^2</f>
-        <v>5.6481172377729036</v>
+        <v>5.6481172907063586</v>
       </c>
       <c r="K37" s="15">
         <f t="shared" ref="K37:K41" si="12">D37*E37/F17^2</f>
-        <v>129.90669646877677</v>
+        <v>129.90669768624625</v>
       </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D38" s="32">
+      <c r="D38" s="31">
         <f t="shared" si="7"/>
         <v>32.9</v>
       </c>
-      <c r="E38" s="39">
+      <c r="E38" s="38">
         <f t="shared" si="7"/>
         <v>32.716666666666669</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38">
         <f t="shared" si="8"/>
-        <v>0.24689664632055416</v>
-      </c>
-      <c r="H38" s="33">
+        <v>0.2492039318842586</v>
+      </c>
+      <c r="H38" s="32">
         <f t="shared" si="9"/>
-        <v>8.1228996639462316</v>
+        <v>8.1988093589921078</v>
       </c>
       <c r="I38" s="15">
         <f>D18^2*G38</f>
-        <v>267.24339894383098</v>
+        <v>269.74082791084032</v>
       </c>
       <c r="J38" s="15">
         <f t="shared" si="11"/>
-        <v>8.0776352787874632</v>
+        <v>8.1531219714799938</v>
       </c>
       <c r="K38" s="15">
         <f t="shared" si="12"/>
-        <v>265.75420067210757</v>
+        <v>268.23771286169182</v>
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D39" s="32">
+      <c r="D39" s="31">
         <f t="shared" si="7"/>
         <v>53.6</v>
       </c>
-      <c r="E39" s="39">
+      <c r="E39" s="38">
         <f t="shared" si="7"/>
         <v>57.6</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39">
         <f t="shared" si="8"/>
-        <v>0.15821783431428393</v>
-      </c>
-      <c r="H39" s="33">
+        <v>0.24070864625457347</v>
+      </c>
+      <c r="H39" s="32">
         <f t="shared" si="9"/>
-        <v>8.4804759192456185</v>
+        <v>12.901983439245138</v>
       </c>
       <c r="I39" s="15">
         <f t="shared" si="10"/>
-        <v>454.55350927156519</v>
+        <v>691.5463123435394</v>
       </c>
       <c r="J39" s="15">
         <f t="shared" si="11"/>
-        <v>9.1133472565027542</v>
+        <v>13.864818024263432</v>
       </c>
       <c r="K39" s="15">
         <f t="shared" si="12"/>
-        <v>488.47541294854761</v>
+        <v>743.15424610052003</v>
       </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.35">
@@ -4149,30 +4001,30 @@
         <f t="shared" si="7"/>
         <v>75.099999999999994</v>
       </c>
-      <c r="E40" s="39">
+      <c r="E40" s="38">
         <f t="shared" si="7"/>
         <v>73.833333333333329</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40">
         <f t="shared" si="8"/>
-        <v>0.24948993169520089</v>
-      </c>
-      <c r="H40" s="33">
+        <v>0.24986396295350308</v>
+      </c>
+      <c r="H40" s="32">
         <f t="shared" si="9"/>
-        <v>18.736693870309587</v>
+        <v>18.764783617808082</v>
       </c>
       <c r="I40" s="15">
         <f t="shared" si="10"/>
-        <v>1407.1257096602499</v>
+        <v>1409.2352496973867</v>
       </c>
       <c r="J40" s="15">
         <f t="shared" si="11"/>
-        <v>18.420673290162334</v>
+        <v>18.448289264733642</v>
       </c>
       <c r="K40" s="15">
         <f t="shared" si="12"/>
-        <v>1383.3925640911909</v>
+        <v>1385.4665237814966</v>
       </c>
     </row>
     <row r="41" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4180,211 +4032,211 @@
         <f t="shared" si="7"/>
         <v>85.18</v>
       </c>
-      <c r="E41" s="39">
+      <c r="E41" s="38">
         <f t="shared" si="7"/>
         <v>83.75</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41">
         <f t="shared" si="8"/>
-        <v>0.24898951754131152</v>
-      </c>
-      <c r="H41" s="33">
+        <v>0.24982928332306256</v>
+      </c>
+      <c r="H41" s="32">
         <f t="shared" si="9"/>
-        <v>21.208927104168918</v>
+        <v>21.280458353458471</v>
       </c>
       <c r="I41" s="15">
         <f t="shared" si="10"/>
-        <v>1806.5764107331086</v>
+        <v>1812.6694425475928</v>
       </c>
       <c r="J41" s="15">
         <f t="shared" si="11"/>
-        <v>20.852872094084841</v>
+        <v>20.923202478306489</v>
       </c>
       <c r="K41" s="15">
         <f t="shared" si="12"/>
-        <v>1776.2476449741469</v>
+        <v>1782.238387102147</v>
       </c>
     </row>
     <row r="42" spans="4:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="36">
+      <c r="G42" s="35">
         <f>SUM(G36:G41)</f>
-        <v>1.4009775231101556</v>
-      </c>
-      <c r="H42" s="17">
+        <v>1.489307426135255</v>
+      </c>
+      <c r="H42" s="16">
         <f>SUM(H36:H41)</f>
-        <v>64.252068992503411</v>
-      </c>
-      <c r="I42" s="18">
+        <v>68.867419506704209</v>
+      </c>
+      <c r="I42" s="17">
         <f>SUM(I36:I41)</f>
-        <v>4083.1493679536052</v>
-      </c>
-      <c r="J42" s="18">
+        <v>4330.9868398463541</v>
+      </c>
+      <c r="J42" s="17">
         <f>SUM(J36:J41)</f>
-        <v>65.086372421288743</v>
-      </c>
-      <c r="K42" s="19">
+        <v>70.039131000570379</v>
+      </c>
+      <c r="K42" s="18">
         <f>SUM(K36:K41)</f>
-        <v>4067.2689645401997</v>
+        <v>4332.7160651036374</v>
       </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D43" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="26">
+      <c r="D43" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="25">
         <f>COUNT(E36:E41)</f>
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="H44" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I44" s="21"/>
-      <c r="K44" s="22"/>
+      <c r="H44" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44" s="20"/>
+      <c r="K44" s="21"/>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.35">
       <c r="H45" s="9">
         <f>G42*I42-H42^2</f>
-        <v>1592.0721181870204</v>
-      </c>
-      <c r="I45" s="22"/>
-      <c r="K45" s="22"/>
+        <v>1707.4493935648525</v>
+      </c>
+      <c r="I45" s="21"/>
+      <c r="K45" s="21"/>
     </row>
     <row r="46" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H46" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
+      <c r="H46" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D47" s="27" t="s">
+      <c r="D47" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="27" t="s">
+      <c r="E47" s="26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D48" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="H48" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I48" s="20" t="s">
-        <v>36</v>
+        <v>13</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="D49" s="39">
+      <c r="D49" s="38">
         <f>E36</f>
         <v>12.016666666666666</v>
       </c>
-      <c r="E49" s="29">
+      <c r="E49" s="28">
         <f>$H$56*D49+$I$56</f>
-        <v>9.6981190489752187</v>
-      </c>
-      <c r="H49" s="35">
+        <v>9.5513194889059019</v>
+      </c>
+      <c r="H49" s="34">
         <f>(1/H45)*(G42*K42-H42*J42)</f>
-        <v>0.95235529292889154</v>
-      </c>
-      <c r="I49" s="34">
+        <v>0.954249069245513</v>
+      </c>
+      <c r="I49" s="33">
         <f>(1/H45)*(I42*J42-H42*K42)</f>
-        <v>2.7806116589206082</v>
-      </c>
-      <c r="J49" s="47"/>
-      <c r="K49" s="48"/>
+        <v>2.9023289343116794</v>
+      </c>
+      <c r="J49" s="46"/>
+      <c r="K49" s="47"/>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D50" s="39">
+      <c r="D50" s="38">
         <f t="shared" ref="D50:D54" si="13">E37</f>
         <v>22.599999999999998</v>
       </c>
-      <c r="E50" s="29">
+      <c r="E50" s="28">
         <f t="shared" ref="E50:E54" si="14">$H$56*D50+$I$56</f>
-        <v>20.810918454736012</v>
+        <v>20.64206474024909</v>
       </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D51" s="39">
+      <c r="D51" s="38">
         <f t="shared" si="13"/>
         <v>32.716666666666669</v>
       </c>
-      <c r="E51" s="29">
+      <c r="E51" s="28">
         <f t="shared" si="14"/>
-        <v>31.433704658353026</v>
+        <v>31.243769256099995</v>
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D52" s="39">
+      <c r="D52" s="38">
         <f t="shared" si="13"/>
         <v>57.6</v>
       </c>
-      <c r="E52" s="29">
+      <c r="E52" s="28">
         <f t="shared" si="14"/>
-        <v>57.561908615519755</v>
+        <v>57.320119902171463</v>
       </c>
     </row>
     <row r="53" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="D53" s="39">
+      <c r="D53" s="38">
         <f t="shared" si="13"/>
         <v>73.833333333333329</v>
       </c>
-      <c r="E53" s="29">
+      <c r="E53" s="28">
         <f t="shared" si="14"/>
-        <v>74.60736786152134</v>
-      </c>
-      <c r="H53" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="49"/>
+        <v>74.331751201082113</v>
+      </c>
+      <c r="H53" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="48"/>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D54" s="39">
+      <c r="D54" s="38">
         <f t="shared" si="13"/>
         <v>83.75</v>
       </c>
-      <c r="E54" s="29">
+      <c r="E54" s="28">
         <f t="shared" si="14"/>
-        <v>85.020148407076732</v>
+        <v>84.72386683029346</v>
       </c>
     </row>
     <row r="55" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H55" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I55" s="24" t="s">
-        <v>34</v>
+      <c r="H55" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E56">
         <v>99.625718693830393</v>
       </c>
-      <c r="H56" s="31">
+      <c r="H56" s="30">
         <f xml:space="preserve"> 1/H49</f>
-        <v>1.0500282903081066</v>
-      </c>
-      <c r="I56" s="30">
+        <v>1.0479444331977819</v>
+      </c>
+      <c r="I56" s="29">
         <f xml:space="preserve"> -I49/H49</f>
-        <v>-2.919720906227194</v>
-      </c>
-      <c r="J56" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K56" s="41"/>
+        <v>-3.0414794500207751</v>
+      </c>
+      <c r="J56" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="K56" s="40"/>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.35">
       <c r="E57">
@@ -4392,178 +4244,7 @@
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="H58" s="31"/>
-    </row>
-    <row r="61" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="G61" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I61" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="K61" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="G62">
-        <f>1/F16^2</f>
-        <v>0.24746690130195087</v>
-      </c>
-      <c r="H62" s="33">
-        <f>D16/F16^2</f>
-        <v>1.9549885202854118</v>
-      </c>
-      <c r="I62" s="15">
-        <f>H62^2</f>
-        <v>3.8219801144477441</v>
-      </c>
-      <c r="J62" s="15">
-        <f>E62</f>
-        <v>0</v>
-      </c>
-      <c r="K62" s="15">
-        <f>H62*J62</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="G63">
-        <f t="shared" ref="G63:G67" si="15">1/F17^2</f>
-        <v>0.24991669193685415</v>
-      </c>
-      <c r="H63" s="33">
-        <f t="shared" ref="H63:H67" si="16">D17/F17^2</f>
-        <v>5.7480839145476459</v>
-      </c>
-      <c r="I63" s="15">
-        <f t="shared" ref="I63:I67" si="17">H63^2</f>
-        <v>33.040468688681386</v>
-      </c>
-      <c r="J63" s="15">
-        <f t="shared" ref="J63:J67" si="18">E63</f>
-        <v>0</v>
-      </c>
-      <c r="K63" s="15">
-        <f t="shared" ref="K63:K67" si="19">H63*J63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="G64">
-        <f t="shared" si="15"/>
-        <v>0.24689664632055416</v>
-      </c>
-      <c r="H64" s="33">
-        <f t="shared" si="16"/>
-        <v>8.1228996639462316</v>
-      </c>
-      <c r="I64" s="15">
-        <f t="shared" si="17"/>
-        <v>65.981498950537798</v>
-      </c>
-      <c r="J64" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K64" s="15">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="7:11" x14ac:dyDescent="0.35">
-      <c r="G65">
-        <f t="shared" si="15"/>
-        <v>0.15821783431428393</v>
-      </c>
-      <c r="H65" s="33">
-        <f t="shared" si="16"/>
-        <v>8.4804759192456185</v>
-      </c>
-      <c r="I65" s="15">
-        <f t="shared" si="17"/>
-        <v>71.918471816904812</v>
-      </c>
-      <c r="J65" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K65" s="15">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="7:11" x14ac:dyDescent="0.35">
-      <c r="G66">
-        <f t="shared" si="15"/>
-        <v>0.24948993169520089</v>
-      </c>
-      <c r="H66" s="33">
-        <f t="shared" si="16"/>
-        <v>18.736693870309587</v>
-      </c>
-      <c r="I66" s="15">
-        <f t="shared" si="17"/>
-        <v>351.06369718969682</v>
-      </c>
-      <c r="J66" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K66" s="15">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G67">
-        <f t="shared" si="15"/>
-        <v>0.24898951754131152</v>
-      </c>
-      <c r="H67" s="33">
-        <f t="shared" si="16"/>
-        <v>21.208927104168918</v>
-      </c>
-      <c r="I67" s="16">
-        <f t="shared" si="17"/>
-        <v>449.81858890995096</v>
-      </c>
-      <c r="J67" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K67" s="16">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="7:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G68">
-        <f>SUM(G62:G67)</f>
-        <v>1.4009775231101556</v>
-      </c>
-      <c r="H68" s="17">
-        <f>SUM(H62:H67)</f>
-        <v>64.252068992503411</v>
-      </c>
-      <c r="I68" s="18">
-        <f>SUM(I62:I67)</f>
-        <v>975.64470567021954</v>
-      </c>
-      <c r="J68" s="18">
-        <f>SUM(J62:J67)</f>
-        <v>0</v>
-      </c>
-      <c r="K68" s="19">
-        <f>SUM(K62:K67)</f>
-        <v>0</v>
-      </c>
+      <c r="H58" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Atualização - Calibragem DHT22
</commit_message>
<xml_diff>
--- a/Calibração DHT-22.xlsx
+++ b/Calibração DHT-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Estacao_meteorologica\Estacao_Meteorologica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD0185E-5C90-43C7-979A-A0D2F6509759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC63C65-EAFA-4482-8045-AE85414713B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Medições da Temperatura</t>
   </si>
@@ -48,76 +48,13 @@
     <t>Y</t>
   </si>
   <si>
-    <r>
-      <t>Δ (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">C </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) :</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> f -1 (y) = 4,6792.y - 8,7631</t>
   </si>
   <si>
     <t xml:space="preserve">nro de leituras (n) : </t>
   </si>
   <si>
-    <t>Ssigma</t>
-  </si>
-  <si>
-    <t>Incerteza  Padrão</t>
-  </si>
-  <si>
     <t xml:space="preserve">Desvio Padrão </t>
-  </si>
-  <si>
-    <t>Incerteza tipoA(V)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incerteza Padrão </t>
   </si>
   <si>
     <t>DHT22 (UR%)</t>
@@ -126,13 +63,7 @@
     <t>URmed(UR%)</t>
   </si>
   <si>
-    <t>Incerteza tipoB(UR%)</t>
-  </si>
-  <si>
     <t>Incerteza tipoB(T)</t>
-  </si>
-  <si>
-    <t>dU/dT</t>
   </si>
   <si>
     <t>UR(%) padrão</t>
@@ -303,7 +234,16 @@
     <t>MMq Umidade. [%]</t>
   </si>
   <si>
-    <t>Sx (%)</t>
+    <t>dU/dT (% / °C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incerteza Padrão ( %) </t>
+  </si>
+  <si>
+    <t>Ssigma(1/(%.%))</t>
+  </si>
+  <si>
+    <t>Sx (1/%)</t>
   </si>
   <si>
     <r>
@@ -330,7 +270,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (% </t>
+      <t xml:space="preserve"> (%.% / (%.%))</t>
+    </r>
+  </si>
+  <si>
+    <t>Sy (1/%)</t>
+  </si>
+  <si>
+    <t>Sxy (% / %)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Δ (1/% </t>
     </r>
     <r>
       <rPr>
@@ -353,14 +304,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)</t>
+      <t>) :</t>
     </r>
   </si>
   <si>
-    <t>Sy (%)</t>
+    <t>Incerteza tipoA(%)</t>
   </si>
   <si>
-    <t>Sxy (% . %)</t>
+    <t>Incerteza tipoB(%)</t>
   </si>
 </sst>
 </file>
@@ -617,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -633,9 +584,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3326,8 +3274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61:K68"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3336,7 +3284,8 @@
     <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="4" max="4" width="21.26953125" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
     <col min="8" max="8" width="19.54296875" customWidth="1"/>
     <col min="9" max="9" width="26.26953125" customWidth="1"/>
     <col min="11" max="11" width="23.54296875" customWidth="1"/>
@@ -3344,63 +3293,65 @@
     <col min="13" max="13" width="15.81640625" customWidth="1"/>
     <col min="14" max="14" width="22.1796875" customWidth="1"/>
     <col min="15" max="15" width="18.7265625" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" customWidth="1"/>
+    <col min="18" max="18" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:25" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:25" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+        <v>10</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="37" t="s">
-        <v>11</v>
+      <c r="P3" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="36" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
         <v>25.9</v>
@@ -3455,7 +3406,7 @@
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>24</v>
@@ -3510,7 +3461,7 @@
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>20.8</v>
@@ -3565,7 +3516,7 @@
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <v>23</v>
@@ -3620,7 +3571,7 @@
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>23.5</v>
@@ -3675,7 +3626,7 @@
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
         <v>23</v>
@@ -3729,25 +3680,25 @@
       <c r="Y9" s="4"/>
     </row>
     <row r="14" spans="2:25" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" spans="2:25" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.35">
@@ -3835,408 +3786,408 @@
       </c>
     </row>
     <row r="34" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
     </row>
     <row r="35" spans="4:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D35" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>36</v>
+        <v>8</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D36" s="31">
+      <c r="D36" s="30">
         <f>D16</f>
         <v>7.9</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="37">
         <f>E16</f>
         <v>12.016666666666666</v>
       </c>
-      <c r="F36" s="14"/>
+      <c r="F36" s="13"/>
       <c r="G36">
         <f>1/(F16^2)</f>
         <v>0.24978490744081483</v>
       </c>
-      <c r="H36" s="32">
+      <c r="H36" s="31">
         <f>D36/F16^2</f>
         <v>1.9733007687824373</v>
       </c>
-      <c r="I36" s="15">
+      <c r="I36" s="14">
         <f>D16^2*G36</f>
         <v>15.589076073381255</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="14">
         <f>E36/F16^2</f>
         <v>3.0015819710804581</v>
       </c>
-      <c r="K36" s="15">
+      <c r="K36" s="14">
         <f>D36*E36/F16^2</f>
         <v>23.712497571535618</v>
       </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D37" s="31">
+      <c r="D37" s="30">
         <f t="shared" ref="D37:E41" si="7">D17</f>
         <v>23</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E37" s="37">
         <f t="shared" si="7"/>
         <v>22.599999999999998</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="13"/>
       <c r="G37">
         <f t="shared" ref="G37:G41" si="8">1/(F17^2)</f>
         <v>0.24991669427904245</v>
       </c>
-      <c r="H37" s="32">
+      <c r="H37" s="31">
         <f t="shared" ref="H37:H41" si="9">D37/F17^2</f>
         <v>5.7480839684179763</v>
       </c>
-      <c r="I37" s="15">
-        <f t="shared" ref="I37:I41" si="10">D17^2*G37</f>
+      <c r="I37" s="14">
+        <f>D17^2*G37</f>
         <v>132.20593127361346</v>
       </c>
-      <c r="J37" s="15">
-        <f t="shared" ref="J37:J41" si="11">E37/F17^2</f>
+      <c r="J37" s="14">
+        <f t="shared" ref="J37:J41" si="10">E37/F17^2</f>
         <v>5.6481172907063586</v>
       </c>
-      <c r="K37" s="15">
-        <f t="shared" ref="K37:K41" si="12">D37*E37/F17^2</f>
+      <c r="K37" s="14">
+        <f t="shared" ref="K37:K41" si="11">D37*E37/F17^2</f>
         <v>129.90669768624625</v>
       </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D38" s="31">
+      <c r="D38" s="30">
         <f t="shared" si="7"/>
         <v>32.9</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="37">
         <f t="shared" si="7"/>
         <v>32.716666666666669</v>
       </c>
-      <c r="F38" s="14"/>
+      <c r="F38" s="13"/>
       <c r="G38">
         <f t="shared" si="8"/>
         <v>0.2492039318842586</v>
       </c>
-      <c r="H38" s="32">
+      <c r="H38" s="31">
         <f t="shared" si="9"/>
         <v>8.1988093589921078</v>
       </c>
-      <c r="I38" s="15">
+      <c r="I38" s="14">
         <f>D18^2*G38</f>
         <v>269.74082791084032</v>
       </c>
-      <c r="J38" s="15">
+      <c r="J38" s="14">
+        <f t="shared" si="10"/>
+        <v>8.1531219714799938</v>
+      </c>
+      <c r="K38" s="14">
         <f t="shared" si="11"/>
-        <v>8.1531219714799938</v>
-      </c>
-      <c r="K38" s="15">
-        <f t="shared" si="12"/>
         <v>268.23771286169182</v>
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D39" s="31">
+      <c r="D39" s="30">
         <f t="shared" si="7"/>
         <v>53.6</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="37">
         <f t="shared" si="7"/>
         <v>57.6</v>
       </c>
-      <c r="F39" s="14"/>
+      <c r="F39" s="13"/>
       <c r="G39">
         <f t="shared" si="8"/>
         <v>0.24070864625457347</v>
       </c>
-      <c r="H39" s="32">
+      <c r="H39" s="31">
         <f t="shared" si="9"/>
         <v>12.901983439245138</v>
       </c>
-      <c r="I39" s="15">
+      <c r="I39" s="14">
+        <f t="shared" ref="I37:I41" si="12">D19^2*G39</f>
+        <v>691.5463123435394</v>
+      </c>
+      <c r="J39" s="14">
         <f t="shared" si="10"/>
-        <v>691.5463123435394</v>
-      </c>
-      <c r="J39" s="15">
+        <v>13.864818024263432</v>
+      </c>
+      <c r="K39" s="14">
         <f t="shared" si="11"/>
-        <v>13.864818024263432</v>
-      </c>
-      <c r="K39" s="15">
-        <f t="shared" si="12"/>
         <v>743.15424610052003</v>
       </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D40" s="13">
+      <c r="D40" s="12">
         <f t="shared" si="7"/>
         <v>75.099999999999994</v>
       </c>
-      <c r="E40" s="38">
+      <c r="E40" s="37">
         <f t="shared" si="7"/>
         <v>73.833333333333329</v>
       </c>
-      <c r="F40" s="14"/>
+      <c r="F40" s="13"/>
       <c r="G40">
         <f t="shared" si="8"/>
         <v>0.24986396295350308</v>
       </c>
-      <c r="H40" s="32">
+      <c r="H40" s="31">
         <f t="shared" si="9"/>
         <v>18.764783617808082</v>
       </c>
-      <c r="I40" s="15">
+      <c r="I40" s="14">
+        <f t="shared" si="12"/>
+        <v>1409.2352496973867</v>
+      </c>
+      <c r="J40" s="14">
         <f t="shared" si="10"/>
-        <v>1409.2352496973867</v>
-      </c>
-      <c r="J40" s="15">
+        <v>18.448289264733642</v>
+      </c>
+      <c r="K40" s="14">
         <f t="shared" si="11"/>
-        <v>18.448289264733642</v>
-      </c>
-      <c r="K40" s="15">
-        <f t="shared" si="12"/>
         <v>1385.4665237814966</v>
       </c>
     </row>
     <row r="41" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D41" s="13">
+      <c r="D41" s="12">
         <f t="shared" si="7"/>
         <v>85.18</v>
       </c>
-      <c r="E41" s="38">
+      <c r="E41" s="37">
         <f t="shared" si="7"/>
         <v>83.75</v>
       </c>
-      <c r="F41" s="14"/>
+      <c r="F41" s="13"/>
       <c r="G41">
         <f t="shared" si="8"/>
         <v>0.24982928332306256</v>
       </c>
-      <c r="H41" s="32">
+      <c r="H41" s="31">
         <f t="shared" si="9"/>
         <v>21.280458353458471</v>
       </c>
-      <c r="I41" s="15">
+      <c r="I41" s="14">
+        <f t="shared" si="12"/>
+        <v>1812.6694425475928</v>
+      </c>
+      <c r="J41" s="14">
         <f t="shared" si="10"/>
-        <v>1812.6694425475928</v>
-      </c>
-      <c r="J41" s="15">
+        <v>20.923202478306489</v>
+      </c>
+      <c r="K41" s="14">
         <f t="shared" si="11"/>
-        <v>20.923202478306489</v>
-      </c>
-      <c r="K41" s="15">
-        <f t="shared" si="12"/>
         <v>1782.238387102147</v>
       </c>
     </row>
     <row r="42" spans="4:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="35">
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="34">
         <f>SUM(G36:G41)</f>
         <v>1.489307426135255</v>
       </c>
-      <c r="H42" s="16">
+      <c r="H42" s="15">
         <f>SUM(H36:H41)</f>
         <v>68.867419506704209</v>
       </c>
-      <c r="I42" s="17">
+      <c r="I42" s="16">
         <f>SUM(I36:I41)</f>
         <v>4330.9868398463541</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J42" s="16">
         <f>SUM(J36:J41)</f>
         <v>70.039131000570379</v>
       </c>
-      <c r="K42" s="18">
+      <c r="K42" s="17">
         <f>SUM(K36:K41)</f>
         <v>4332.7160651036374</v>
       </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D43" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="25">
+      <c r="D43" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="24">
         <f>COUNT(E36:E41)</f>
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="H44" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="I44" s="20"/>
-      <c r="K44" s="21"/>
+      <c r="H44" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I44" s="19"/>
+      <c r="K44" s="20"/>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="H45" s="9">
+      <c r="H45" s="8">
         <f>G42*I42-H42^2</f>
         <v>1707.4493935648525</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="K45" s="21"/>
+      <c r="I45" s="20"/>
+      <c r="K45" s="20"/>
     </row>
     <row r="46" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H46" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
+      <c r="H46" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="26" t="s">
+      <c r="E47" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="4:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D48" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="H48" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="19" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I48" s="18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="D49" s="38">
+      <c r="D49" s="37">
         <f>E36</f>
         <v>12.016666666666666</v>
       </c>
-      <c r="E49" s="28">
+      <c r="E49" s="27">
         <f>$H$56*D49+$I$56</f>
         <v>9.5513194889059019</v>
       </c>
-      <c r="H49" s="34">
+      <c r="H49" s="33">
         <f>(1/H45)*(G42*K42-H42*J42)</f>
         <v>0.954249069245513</v>
       </c>
-      <c r="I49" s="33">
+      <c r="I49" s="32">
         <f>(1/H45)*(I42*J42-H42*K42)</f>
         <v>2.9023289343116794</v>
       </c>
-      <c r="J49" s="46"/>
-      <c r="K49" s="47"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="46"/>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D50" s="38">
+      <c r="D50" s="37">
         <f t="shared" ref="D50:D54" si="13">E37</f>
         <v>22.599999999999998</v>
       </c>
-      <c r="E50" s="28">
+      <c r="E50" s="27">
         <f t="shared" ref="E50:E54" si="14">$H$56*D50+$I$56</f>
         <v>20.64206474024909</v>
       </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D51" s="38">
+      <c r="D51" s="37">
         <f t="shared" si="13"/>
         <v>32.716666666666669</v>
       </c>
-      <c r="E51" s="28">
+      <c r="E51" s="27">
         <f t="shared" si="14"/>
         <v>31.243769256099995</v>
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D52" s="38">
+      <c r="D52" s="37">
         <f t="shared" si="13"/>
         <v>57.6</v>
       </c>
-      <c r="E52" s="28">
+      <c r="E52" s="27">
         <f t="shared" si="14"/>
         <v>57.320119902171463</v>
       </c>
     </row>
     <row r="53" spans="4:11" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="D53" s="38">
+      <c r="D53" s="37">
         <f t="shared" si="13"/>
         <v>73.833333333333329</v>
       </c>
-      <c r="E53" s="28">
+      <c r="E53" s="27">
         <f t="shared" si="14"/>
         <v>74.331751201082113</v>
       </c>
-      <c r="H53" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="I53" s="48"/>
-      <c r="J53" s="48"/>
-      <c r="K53" s="48"/>
+      <c r="H53" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="I53" s="47"/>
+      <c r="J53" s="47"/>
+      <c r="K53" s="47"/>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D54" s="38">
+      <c r="D54" s="37">
         <f t="shared" si="13"/>
         <v>83.75</v>
       </c>
-      <c r="E54" s="28">
+      <c r="E54" s="27">
         <f t="shared" si="14"/>
         <v>84.72386683029346</v>
       </c>
     </row>
     <row r="55" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H55" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I55" s="23" t="s">
-        <v>27</v>
+      <c r="H55" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="22" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E56">
         <v>99.625718693830393</v>
       </c>
-      <c r="H56" s="30">
+      <c r="H56" s="29">
         <f xml:space="preserve"> 1/H49</f>
         <v>1.0479444331977819</v>
       </c>
-      <c r="I56" s="29">
+      <c r="I56" s="28">
         <f xml:space="preserve"> -I49/H49</f>
         <v>-3.0414794500207751</v>
       </c>
-      <c r="J56" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="K56" s="40"/>
+      <c r="J56" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="K56" s="39"/>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.35">
       <c r="E57">
@@ -4244,7 +4195,7 @@
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="H58" s="30"/>
+      <c r="H58" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>